<commit_message>
- Ajouté des fichiers de paroisses pour l'importation.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@21161 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Région 3/id.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Région 3/id.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>_id</t>
   </si>
@@ -46,6 +46,21 @@
   </si>
   <si>
     <t>Prilly – Jouxtens</t>
+  </si>
+  <si>
+    <t>Les Chamberonnes</t>
+  </si>
+  <si>
+    <t>Le Mont-sur-Lausanne</t>
+  </si>
+  <si>
+    <t>Ecublens – Saint-Sulpice</t>
+  </si>
+  <si>
+    <t>Renens</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -89,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -98,9 +113,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -442,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -480,19 +492,19 @@
       <c r="A2" s="2">
         <v>2</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>3040000000</v>
       </c>
       <c r="C2" s="3">
         <v>3040</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>3000</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>1</v>
       </c>
       <c r="G2" t="s">
@@ -500,12 +512,96 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>3000000000</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3000</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3030000000</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3030</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>3080000000</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3080</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>3090000000</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3090</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
- Rajouté les fichiers de 4 paroisses.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@21332 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Région 3/id.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Région 3/id.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>_id</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>Bussigny – Villars-Sainte-Croix</t>
   </si>
 </sst>
 </file>
@@ -454,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -603,6 +606,29 @@
         <v>7</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>3050000000</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3050</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>